<commit_message>
en la misma linea que el commit anterior
</commit_message>
<xml_diff>
--- a/results/complete_table.xlsx
+++ b/results/complete_table.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="28">
   <si>
     <t>Parameter</t>
   </si>
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -143,11 +143,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -167,6 +169,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -195,53 +199,53 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="19" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -282,7 +286,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -323,12 +327,12 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B6">
@@ -357,7 +361,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B7">
@@ -386,7 +390,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C8">
@@ -403,7 +407,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C9">
@@ -420,7 +424,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C10">
@@ -437,7 +441,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C11">
@@ -454,7 +458,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D12">
@@ -471,7 +475,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
       <c r="H13">
@@ -485,27 +489,27 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B18">

</xml_diff>

<commit_message>
en esta versión hice dos cosas, agregué los calculos de ll marginales y ll copulas que aparecen al final de la tabla, y agregué al principio de la tabla los parámetros marginales
</commit_message>
<xml_diff>
--- a/results/complete_table.xlsx
+++ b/results/complete_table.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="28">
   <si>
     <t>Parameter</t>
   </si>
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -145,11 +145,21 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -171,6 +181,16 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -189,63 +209,63 @@
     <col min="4" max="4" width="9.33203125" customWidth="true"/>
     <col min="5" max="5" width="14" customWidth="true"/>
     <col min="6" max="6" width="16.21875" customWidth="true"/>
-    <col min="7" max="7" width="11.21875" customWidth="true"/>
+    <col min="7" max="7" width="12.21875" customWidth="true"/>
     <col min="8" max="8" width="15.21875" customWidth="true"/>
     <col min="9" max="9" width="17.44140625" customWidth="true"/>
     <col min="10" max="10" width="12.44140625" customWidth="true"/>
     <col min="11" max="11" width="11.44140625" customWidth="true"/>
     <col min="12" max="12" width="13.6640625" customWidth="true"/>
-    <col min="13" max="13" width="8.6640625" customWidth="true"/>
+    <col min="13" max="13" width="9.21875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="29" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -286,7 +306,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -327,12 +347,12 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="29" t="s">
         <v>2</v>
       </c>
       <c r="B6">
@@ -361,7 +381,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B7">
@@ -390,7 +410,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C8">
@@ -407,7 +427,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C9">
@@ -424,7 +444,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C10">
@@ -441,7 +461,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C11">
@@ -458,7 +478,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="29" t="s">
         <v>9</v>
       </c>
       <c r="D12">
@@ -475,7 +495,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="29" t="s">
         <v>10</v>
       </c>
       <c r="H13">
@@ -489,27 +509,135 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="29" t="s">
         <v>12</v>
       </c>
+      <c r="B15">
+        <v>-2939.1999999999998</v>
+      </c>
+      <c r="C15">
+        <v>-2939.1999999999998</v>
+      </c>
+      <c r="D15">
+        <v>-3132.0479999999998</v>
+      </c>
+      <c r="E15">
+        <v>-3055.0430000000001</v>
+      </c>
+      <c r="F15">
+        <v>-3056.8409999999999</v>
+      </c>
+      <c r="G15">
+        <v>-3151.2579999999998</v>
+      </c>
+      <c r="H15">
+        <v>-543824.09100000001</v>
+      </c>
+      <c r="I15">
+        <v>-543824.09100000001</v>
+      </c>
+      <c r="J15">
+        <v>-4336168.7170000002</v>
+      </c>
+      <c r="K15">
+        <v>-5964.6729999999998</v>
+      </c>
+      <c r="L15">
+        <v>-5964.6729999999998</v>
+      </c>
+      <c r="M15">
+        <v>-5964.6729999999998</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="29" t="s">
         <v>13</v>
       </c>
+      <c r="B16">
+        <v>-2989.895</v>
+      </c>
+      <c r="C16">
+        <v>-2989.895</v>
+      </c>
+      <c r="D16">
+        <v>-3125.98</v>
+      </c>
+      <c r="E16">
+        <v>-2888.8539999999998</v>
+      </c>
+      <c r="F16">
+        <v>-2893.4520000000002</v>
+      </c>
+      <c r="G16">
+        <v>-3117.2359999999999</v>
+      </c>
+      <c r="H16">
+        <v>-544279.91700000002</v>
+      </c>
+      <c r="I16">
+        <v>-544279.91799999995</v>
+      </c>
+      <c r="J16">
+        <v>-4496945.9809999997</v>
+      </c>
+      <c r="K16">
+        <v>-4153.8540000000003</v>
+      </c>
+      <c r="L16">
+        <v>-4153.8540000000003</v>
+      </c>
+      <c r="M16">
+        <v>-4153.8540000000003</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="29" t="s">
         <v>14</v>
       </c>
+      <c r="B17">
+        <v>-424.99599999999998</v>
+      </c>
+      <c r="C17">
+        <v>-424.99599999999998</v>
+      </c>
+      <c r="D17">
+        <v>-100.97</v>
+      </c>
+      <c r="E17">
+        <v>-352.38999999999999</v>
+      </c>
+      <c r="F17">
+        <v>-404.56200000000001</v>
+      </c>
+      <c r="G17">
+        <v>-2030816.2949999999</v>
+      </c>
+      <c r="H17">
+        <v>1064236.9099999999</v>
+      </c>
+      <c r="I17">
+        <v>1064227.1470000001</v>
+      </c>
+      <c r="J17">
+        <v>8807701.3900000006</v>
+      </c>
+      <c r="K17">
+        <v>871.09000000000003</v>
+      </c>
+      <c r="L17">
+        <v>871.09000000000003</v>
+      </c>
+      <c r="M17">
+        <v>1057.864</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B18">

</xml_diff>

<commit_message>
enviada esta versión al cliente
</commit_message>
<xml_diff>
--- a/results/complete_table.xlsx
+++ b/results/complete_table.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="32">
   <si>
     <t>Parameter</t>
   </si>
@@ -129,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -169,11 +169,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -207,6 +209,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -225,7 +229,7 @@
     <col min="4" max="4" width="9.33203125" customWidth="true"/>
     <col min="5" max="5" width="14" customWidth="true"/>
     <col min="6" max="6" width="16.21875" customWidth="true"/>
-    <col min="7" max="7" width="11.6640625" customWidth="true"/>
+    <col min="7" max="7" width="16.21875" customWidth="true"/>
     <col min="8" max="8" width="15.21875" customWidth="true"/>
     <col min="9" max="9" width="17.44140625" customWidth="true"/>
     <col min="10" max="10" width="12.44140625" customWidth="true"/>
@@ -235,53 +239,53 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31" t="s">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="M1" s="33" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>28</v>
       </c>
       <c r="K3">
@@ -295,7 +299,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="33" t="s">
         <v>29</v>
       </c>
       <c r="K4">
@@ -309,7 +313,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
       <c r="K5">
@@ -323,7 +327,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="33" t="s">
         <v>31</v>
       </c>
       <c r="K6">
@@ -337,12 +341,12 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="33" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="33" t="s">
         <v>2</v>
       </c>
       <c r="B8">
@@ -355,7 +359,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.0040000000000000001</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0.012999999999999999</v>
@@ -371,7 +375,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B9">
@@ -381,10 +385,10 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.98999999999999999</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="G9">
-        <v>0.0030000000000000001</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0.98699999999999999</v>
@@ -400,7 +404,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C10">
@@ -417,7 +421,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="33" t="s">
         <v>6</v>
       </c>
       <c r="C11">
@@ -434,7 +438,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="33" t="s">
         <v>7</v>
       </c>
       <c r="C12">
@@ -451,14 +455,14 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="33" t="s">
         <v>8</v>
       </c>
       <c r="C13">
         <v>0.90000000000000002</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="I13">
         <v>0.98999999999999999</v>
@@ -468,14 +472,14 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="33" t="s">
         <v>9</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0.999</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -485,7 +489,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="33" t="s">
         <v>10</v>
       </c>
       <c r="H15">
@@ -499,12 +503,12 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="33" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="33" t="s">
         <v>12</v>
       </c>
       <c r="B17">
@@ -517,13 +521,13 @@
         <v>-3132.0479999999998</v>
       </c>
       <c r="E17">
-        <v>-3055.0430000000001</v>
+        <v>-3059.9540000000002</v>
       </c>
       <c r="F17">
-        <v>-3056.8409999999999</v>
+        <v>-3059.9540000000002</v>
       </c>
       <c r="G17">
-        <v>-3151.252</v>
+        <v>-109265021298.28999</v>
       </c>
       <c r="H17">
         <v>-543824.09100000001</v>
@@ -545,7 +549,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B18">
@@ -558,13 +562,13 @@
         <v>-3125.98</v>
       </c>
       <c r="E18">
-        <v>-2888.8539999999998</v>
+        <v>-2863.9119999999998</v>
       </c>
       <c r="F18">
-        <v>-2893.4520000000002</v>
+        <v>-2863.9119999999998</v>
       </c>
       <c r="G18">
-        <v>-3117.2199999999998</v>
+        <v>-105945556394.51401</v>
       </c>
       <c r="H18">
         <v>-544279.91700000002</v>
@@ -586,7 +590,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="33" t="s">
         <v>14</v>
       </c>
       <c r="B19">
@@ -599,19 +603,19 @@
         <v>-100.971</v>
       </c>
       <c r="E19">
-        <v>-352.38999999999999</v>
+        <v>-430.22500000000002</v>
       </c>
       <c r="F19">
-        <v>-404.56200000000001</v>
+        <v>-430.22500000000002</v>
       </c>
       <c r="G19">
-        <v>-1261928757.6429999</v>
+        <v>215210571333.80499</v>
       </c>
       <c r="H19">
         <v>1064236.9099999999</v>
       </c>
       <c r="I19">
-        <v>1064227.1470000001</v>
+        <v>1064227.1839999999</v>
       </c>
       <c r="J19">
         <v>8807701.3900000006</v>
@@ -627,7 +631,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B20">
@@ -640,19 +644,19 @@
         <v>-6358.9989999999998</v>
       </c>
       <c r="E20">
-        <v>-6296.2870000000003</v>
+        <v>-6354.0919999999996</v>
       </c>
       <c r="F20">
-        <v>-6354.8549999999996</v>
+        <v>-6354.0919999999996</v>
       </c>
       <c r="G20">
-        <v>-1261935026.1140001</v>
+        <v>-6358.9989999999998</v>
       </c>
       <c r="H20">
         <v>-23867.098000000002</v>
       </c>
       <c r="I20">
-        <v>-23876.862000000001</v>
+        <v>-23876.825000000001</v>
       </c>
       <c r="J20">
         <v>-25413.308000000001</v>

</xml_diff>

<commit_message>
agregué un archivo run para correr las tablas 2,4 y 5. No recomendable porque se ralentiza mucho la ejecución del código
</commit_message>
<xml_diff>
--- a/results/complete_table.xlsx
+++ b/results/complete_table.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="32">
   <si>
     <t>Parameter</t>
   </si>
@@ -129,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -171,11 +171,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -211,6 +215,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,53 +247,53 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33" t="s">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="M1" s="37" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="37" t="s">
         <v>28</v>
       </c>
       <c r="K3">
@@ -299,7 +307,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="37" t="s">
         <v>29</v>
       </c>
       <c r="K4">
@@ -313,7 +321,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="37" t="s">
         <v>30</v>
       </c>
       <c r="K5">
@@ -327,7 +335,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="37" t="s">
         <v>31</v>
       </c>
       <c r="K6">
@@ -341,12 +349,12 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="37" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="37" t="s">
         <v>2</v>
       </c>
       <c r="B8">
@@ -375,7 +383,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="37" t="s">
         <v>3</v>
       </c>
       <c r="B9">
@@ -404,7 +412,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="37" t="s">
         <v>5</v>
       </c>
       <c r="C10">
@@ -421,7 +429,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C11">
@@ -438,7 +446,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C12">
@@ -455,7 +463,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="37" t="s">
         <v>8</v>
       </c>
       <c r="C13">
@@ -472,7 +480,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="37" t="s">
         <v>9</v>
       </c>
       <c r="D14">
@@ -489,7 +497,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="37" t="s">
         <v>10</v>
       </c>
       <c r="H15">
@@ -503,12 +511,12 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="37" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="37" t="s">
         <v>12</v>
       </c>
       <c r="B17">
@@ -549,7 +557,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="37" t="s">
         <v>13</v>
       </c>
       <c r="B18">
@@ -590,7 +598,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B19">
@@ -631,7 +639,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B20">

</xml_diff>